<commit_message>
git commit -m "implementação da funcionalidade de imprimir via planilha"
</commit_message>
<xml_diff>
--- a/planilha.xlsx
+++ b/planilha.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://samarces-my.sharepoint.com/personal/joabe_alves_samarces_onmicrosoft_com/Documents/Imprimir Cod Produtos Programa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{58570641-C1DC-485F-8946-D670B9D9F971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{58570641-C1DC-485F-8946-D670B9D9F971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{79A429C6-9E0C-4662-8BBA-0E60E80525C4}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{2E78F4F2-A7A9-45FA-B693-BEF4BCC6E860}"/>
+    <workbookView xWindow="6150" yWindow="3150" windowWidth="21600" windowHeight="11295" xr2:uid="{2E78F4F2-A7A9-45FA-B693-BEF4BCC6E860}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>texto</t>
   </si>
@@ -44,24 +44,26 @@
     <t>quantidade</t>
   </si>
   <si>
-    <t>teste1</t>
+    <t>abcd</t>
   </si>
   <si>
-    <t>teste2</t>
-  </si>
-  <si>
-    <t>teste3</t>
-  </si>
-  <si>
-    <t>testando</t>
+    <t>efgh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -89,8 +91,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D31DE2DB-953B-4DFE-95E8-2B476020F7DE}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,27 +456,12 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>